<commit_message>
Calcul des recrues de troupes pendant l'aller-retour évité par la capture de donjon
</commit_message>
<xml_diff>
--- a/docs/economie-capture.xlsx
+++ b/docs/economie-capture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\Documents\GitHub\Donjons-et-Barons\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2361D2-DD26-4E6D-BBFD-5756E98BEBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650FC2D2-1822-4888-91A4-17269CE99EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>#tours</t>
   </si>
@@ -49,13 +49,19 @@
   <si>
     <t>Recrut. Moy.</t>
   </si>
+  <si>
+    <t>#Troupes</t>
+  </si>
+  <si>
+    <t>Recrut. Bilan</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -187,17 +193,20 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -479,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,24 +499,32 @@
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
+      <c r="F2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="10"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -519,8 +536,15 @@
         <f>B4*C4</f>
         <v>0.22222222222222221</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <f>F4*C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3">
         <v>3</v>
       </c>
@@ -532,8 +556,15 @@
         <f t="shared" ref="D5:D18" si="1">B5*C5</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="3">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" ref="G5:G18" si="2">F5*C5</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3">
         <v>3</v>
       </c>
@@ -545,8 +576,16 @@
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="3">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="2"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3">
         <v>3</v>
       </c>
@@ -558,8 +597,15 @@
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3">
         <v>3</v>
       </c>
@@ -571,8 +617,15 @@
         <f t="shared" si="1"/>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>4</v>
       </c>
@@ -584,8 +637,15 @@
         <f t="shared" si="1"/>
         <v>0.44444444444444442</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -597,113 +657,177 @@
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5">
         <v>3</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" ref="C11:C18" si="2">1/27</f>
+        <f t="shared" ref="C11:C18" si="3">1/27</f>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="6">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="2"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>3</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="5">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7037037037037035E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5">
         <v>3</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>4</v>
       </c>
       <c r="C15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="6">
+        <v>2</v>
+      </c>
+      <c r="G15" s="1">
+        <f t="shared" si="2"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>3</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="1"/>
         <v>0.1111111111111111</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="6">
         <v>4</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="6">
+        <v>2</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="2"/>
+        <v>7.407407407407407E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="6">
         <v>4</v>
       </c>
       <c r="C18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="1"/>
         <v>0.14814814814814814</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="9">
+      <c r="F18" s="6">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G18" s="1">
+        <f t="shared" si="2"/>
+        <v>2.4691358024691357E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="7">
         <f>SUM(C4:C18)</f>
         <v>0.99999999999999956</v>
       </c>
@@ -712,28 +836,43 @@
         <v>3.1481481481481479</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <f>D19/C19</f>
         <v>3.1481481481481493</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="11">
+        <f>SUM(G4:G18)</f>
+        <v>0.83950617283950624</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="8">
         <f>2*B20</f>
         <v>6.2962962962962985</v>
       </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="11">
+        <f>B21-G20</f>
+        <v>5.4567901234567922</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
+    <mergeCell ref="F2:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>